<commit_message>
exportar a sqllite, json, iloc, loc
</commit_message>
<xml_diff>
--- a/03-pandas/Data/mi_df_colores.xlsx
+++ b/03-pandas/Data/mi_df_colores.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Artistas" sheetId="1" r:id="rId1"/>
-    <sheet name="Grafico" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>artist</t>
   </si>
@@ -432,46 +431,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>